<commit_message>
Ran complete tests on opnemp
</commit_message>
<xml_diff>
--- a/coursework 2/code/results.xlsx
+++ b/coursework 2/code/results.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Analysis" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenMP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t>Number of Particles</t>
   </si>
@@ -42,6 +43,12 @@
   </si>
   <si>
     <t>Average Framerate</t>
+  </si>
+  <si>
+    <t>OpenMP</t>
+  </si>
+  <si>
+    <t>Framerate</t>
   </si>
 </sst>
 </file>
@@ -2085,6 +2092,732 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="489178664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>OpenMP!$B$2:$S$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3750</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4250</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>OpenMP!$B$13:$S$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>935.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1399.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2452.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3589.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4911.1000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6471</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8201.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10156.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12303.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14660.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17427.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20446</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23765.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27623.599999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>31402.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>35260.400000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>39282.9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43734</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A99-41FF-AC59-8A52A33DA9C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="509240696"/>
+        <c:axId val="509243648"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="509240696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="509243648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="509243648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="509240696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>OpenMP!$B$2:$S$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3750</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4250</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>OpenMP!$B$14:$S$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1A4E-4C9A-AA24-9EC50DF84D85}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="509221344"/>
+        <c:axId val="509218064"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="509221344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="509218064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="509218064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="509221344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2373,6 +3106,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4954,6 +5767,1038 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5654,6 +7499,71 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>490537</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>185737</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5919,7 +7829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -6894,4 +8804,813 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>250</v>
+      </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="D2">
+        <v>750</v>
+      </c>
+      <c r="E2">
+        <v>1000</v>
+      </c>
+      <c r="F2">
+        <v>1250</v>
+      </c>
+      <c r="G2">
+        <v>1500</v>
+      </c>
+      <c r="H2">
+        <v>1750</v>
+      </c>
+      <c r="I2">
+        <v>2000</v>
+      </c>
+      <c r="J2">
+        <v>2250</v>
+      </c>
+      <c r="K2">
+        <v>2500</v>
+      </c>
+      <c r="L2">
+        <v>2750</v>
+      </c>
+      <c r="M2">
+        <v>3000</v>
+      </c>
+      <c r="N2">
+        <v>3250</v>
+      </c>
+      <c r="O2">
+        <v>3500</v>
+      </c>
+      <c r="P2">
+        <v>3750</v>
+      </c>
+      <c r="Q2">
+        <v>4000</v>
+      </c>
+      <c r="R2">
+        <v>4250</v>
+      </c>
+      <c r="S2">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>917</v>
+      </c>
+      <c r="C3">
+        <v>1361</v>
+      </c>
+      <c r="D3">
+        <v>2506</v>
+      </c>
+      <c r="E3">
+        <v>3724</v>
+      </c>
+      <c r="F3">
+        <v>4905</v>
+      </c>
+      <c r="G3">
+        <v>6447</v>
+      </c>
+      <c r="H3">
+        <v>8134</v>
+      </c>
+      <c r="I3">
+        <v>10195</v>
+      </c>
+      <c r="J3">
+        <v>12378</v>
+      </c>
+      <c r="K3">
+        <v>15016</v>
+      </c>
+      <c r="L3">
+        <v>17343</v>
+      </c>
+      <c r="M3">
+        <v>20423</v>
+      </c>
+      <c r="N3">
+        <v>23802</v>
+      </c>
+      <c r="O3">
+        <v>27455</v>
+      </c>
+      <c r="P3">
+        <v>31215</v>
+      </c>
+      <c r="Q3">
+        <v>35047</v>
+      </c>
+      <c r="R3">
+        <v>39197</v>
+      </c>
+      <c r="S3">
+        <v>43686</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>945</v>
+      </c>
+      <c r="C4">
+        <v>1412</v>
+      </c>
+      <c r="D4">
+        <v>2480</v>
+      </c>
+      <c r="E4">
+        <v>3754</v>
+      </c>
+      <c r="F4">
+        <v>4973</v>
+      </c>
+      <c r="G4">
+        <v>6484</v>
+      </c>
+      <c r="H4">
+        <v>8305</v>
+      </c>
+      <c r="I4">
+        <v>10139</v>
+      </c>
+      <c r="J4">
+        <v>12246</v>
+      </c>
+      <c r="K4">
+        <v>14642</v>
+      </c>
+      <c r="L4">
+        <v>17370</v>
+      </c>
+      <c r="M4">
+        <v>20421</v>
+      </c>
+      <c r="N4">
+        <v>23788</v>
+      </c>
+      <c r="O4">
+        <v>27558</v>
+      </c>
+      <c r="P4">
+        <v>31527</v>
+      </c>
+      <c r="Q4">
+        <v>35223</v>
+      </c>
+      <c r="R4">
+        <v>39086</v>
+      </c>
+      <c r="S4">
+        <v>43695</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1008</v>
+      </c>
+      <c r="C5">
+        <v>1430</v>
+      </c>
+      <c r="D5">
+        <v>2477</v>
+      </c>
+      <c r="E5">
+        <v>3524</v>
+      </c>
+      <c r="F5">
+        <v>4900</v>
+      </c>
+      <c r="G5">
+        <v>6514</v>
+      </c>
+      <c r="H5">
+        <v>8373</v>
+      </c>
+      <c r="I5">
+        <v>10110</v>
+      </c>
+      <c r="J5">
+        <v>12245</v>
+      </c>
+      <c r="K5">
+        <v>14599</v>
+      </c>
+      <c r="L5">
+        <v>17376</v>
+      </c>
+      <c r="M5">
+        <v>20316</v>
+      </c>
+      <c r="N5">
+        <v>23594</v>
+      </c>
+      <c r="O5">
+        <v>27230</v>
+      </c>
+      <c r="P5">
+        <v>31150</v>
+      </c>
+      <c r="Q5">
+        <v>35259</v>
+      </c>
+      <c r="R5">
+        <v>39111</v>
+      </c>
+      <c r="S5">
+        <v>43694</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>905</v>
+      </c>
+      <c r="C6">
+        <v>1627</v>
+      </c>
+      <c r="D6">
+        <v>2477</v>
+      </c>
+      <c r="E6">
+        <v>3521</v>
+      </c>
+      <c r="F6">
+        <v>4898</v>
+      </c>
+      <c r="G6">
+        <v>6524</v>
+      </c>
+      <c r="H6">
+        <v>8332</v>
+      </c>
+      <c r="I6">
+        <v>10116</v>
+      </c>
+      <c r="J6">
+        <v>12246</v>
+      </c>
+      <c r="K6">
+        <v>14659</v>
+      </c>
+      <c r="L6">
+        <v>17373</v>
+      </c>
+      <c r="M6">
+        <v>20318</v>
+      </c>
+      <c r="N6">
+        <v>23712</v>
+      </c>
+      <c r="O6">
+        <v>27415</v>
+      </c>
+      <c r="P6">
+        <v>31475</v>
+      </c>
+      <c r="Q6">
+        <v>35212</v>
+      </c>
+      <c r="R6">
+        <v>39649</v>
+      </c>
+      <c r="S6">
+        <v>43612</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>929</v>
+      </c>
+      <c r="C7">
+        <v>893</v>
+      </c>
+      <c r="D7">
+        <v>2480</v>
+      </c>
+      <c r="E7">
+        <v>4103</v>
+      </c>
+      <c r="F7">
+        <v>4906</v>
+      </c>
+      <c r="G7">
+        <v>6457</v>
+      </c>
+      <c r="H7">
+        <v>8221</v>
+      </c>
+      <c r="I7">
+        <v>10169</v>
+      </c>
+      <c r="J7">
+        <v>12242</v>
+      </c>
+      <c r="K7">
+        <v>14633</v>
+      </c>
+      <c r="L7">
+        <v>17610</v>
+      </c>
+      <c r="M7">
+        <v>20240</v>
+      </c>
+      <c r="N7">
+        <v>23638</v>
+      </c>
+      <c r="O7">
+        <v>27505</v>
+      </c>
+      <c r="P7">
+        <v>31385</v>
+      </c>
+      <c r="Q7">
+        <v>35213</v>
+      </c>
+      <c r="R7">
+        <v>39238</v>
+      </c>
+      <c r="S7">
+        <v>43560</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>901</v>
+      </c>
+      <c r="C8">
+        <v>733</v>
+      </c>
+      <c r="D8">
+        <v>2397</v>
+      </c>
+      <c r="E8">
+        <v>3472</v>
+      </c>
+      <c r="F8">
+        <v>4911</v>
+      </c>
+      <c r="G8">
+        <v>6424</v>
+      </c>
+      <c r="H8">
+        <v>8133</v>
+      </c>
+      <c r="I8">
+        <v>10075</v>
+      </c>
+      <c r="J8">
+        <v>12676</v>
+      </c>
+      <c r="K8">
+        <v>14615</v>
+      </c>
+      <c r="L8">
+        <v>17391</v>
+      </c>
+      <c r="M8">
+        <v>20881</v>
+      </c>
+      <c r="N8">
+        <v>23633</v>
+      </c>
+      <c r="O8">
+        <v>27341</v>
+      </c>
+      <c r="P8">
+        <v>31487</v>
+      </c>
+      <c r="Q8">
+        <v>35090</v>
+      </c>
+      <c r="R8">
+        <v>39340</v>
+      </c>
+      <c r="S8">
+        <v>43975</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>959</v>
+      </c>
+      <c r="C9">
+        <v>1517</v>
+      </c>
+      <c r="D9">
+        <v>2448</v>
+      </c>
+      <c r="E9">
+        <v>3443</v>
+      </c>
+      <c r="F9">
+        <v>4904</v>
+      </c>
+      <c r="G9">
+        <v>6496</v>
+      </c>
+      <c r="H9">
+        <v>8103</v>
+      </c>
+      <c r="I9">
+        <v>10152</v>
+      </c>
+      <c r="J9">
+        <v>12223</v>
+      </c>
+      <c r="K9">
+        <v>14614</v>
+      </c>
+      <c r="L9">
+        <v>17348</v>
+      </c>
+      <c r="M9">
+        <v>20568</v>
+      </c>
+      <c r="N9">
+        <v>23801</v>
+      </c>
+      <c r="O9">
+        <v>27572</v>
+      </c>
+      <c r="P9">
+        <v>31104</v>
+      </c>
+      <c r="Q9">
+        <v>35821</v>
+      </c>
+      <c r="R9">
+        <v>39234</v>
+      </c>
+      <c r="S9">
+        <v>43682</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>934</v>
+      </c>
+      <c r="C10">
+        <v>1407</v>
+      </c>
+      <c r="D10">
+        <v>2428</v>
+      </c>
+      <c r="E10">
+        <v>3486</v>
+      </c>
+      <c r="F10">
+        <v>4927</v>
+      </c>
+      <c r="G10">
+        <v>6482</v>
+      </c>
+      <c r="H10">
+        <v>8090</v>
+      </c>
+      <c r="I10">
+        <v>10079</v>
+      </c>
+      <c r="J10">
+        <v>12237</v>
+      </c>
+      <c r="K10">
+        <v>14635</v>
+      </c>
+      <c r="L10">
+        <v>17571</v>
+      </c>
+      <c r="M10">
+        <v>20439</v>
+      </c>
+      <c r="N10">
+        <v>23812</v>
+      </c>
+      <c r="O10">
+        <v>27398</v>
+      </c>
+      <c r="P10">
+        <v>31415</v>
+      </c>
+      <c r="Q10">
+        <v>35372</v>
+      </c>
+      <c r="R10">
+        <v>39293</v>
+      </c>
+      <c r="S10">
+        <v>43989</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>948</v>
+      </c>
+      <c r="C11">
+        <v>2129</v>
+      </c>
+      <c r="D11">
+        <v>2462</v>
+      </c>
+      <c r="E11">
+        <v>3423</v>
+      </c>
+      <c r="F11">
+        <v>4886</v>
+      </c>
+      <c r="G11">
+        <v>6428</v>
+      </c>
+      <c r="H11">
+        <v>8173</v>
+      </c>
+      <c r="I11">
+        <v>10091</v>
+      </c>
+      <c r="J11">
+        <v>12256</v>
+      </c>
+      <c r="K11">
+        <v>14600</v>
+      </c>
+      <c r="L11">
+        <v>17454</v>
+      </c>
+      <c r="M11">
+        <v>20539</v>
+      </c>
+      <c r="N11">
+        <v>24187</v>
+      </c>
+      <c r="O11">
+        <v>27577</v>
+      </c>
+      <c r="P11">
+        <v>31744</v>
+      </c>
+      <c r="Q11">
+        <v>35242</v>
+      </c>
+      <c r="R11">
+        <v>39134</v>
+      </c>
+      <c r="S11">
+        <v>43713</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>908</v>
+      </c>
+      <c r="C12">
+        <v>1485</v>
+      </c>
+      <c r="D12">
+        <v>2369</v>
+      </c>
+      <c r="E12">
+        <v>3449</v>
+      </c>
+      <c r="F12">
+        <v>4901</v>
+      </c>
+      <c r="G12">
+        <v>6454</v>
+      </c>
+      <c r="H12">
+        <v>8155</v>
+      </c>
+      <c r="I12">
+        <v>10436</v>
+      </c>
+      <c r="J12">
+        <v>12283</v>
+      </c>
+      <c r="K12">
+        <v>14595</v>
+      </c>
+      <c r="L12">
+        <v>17437</v>
+      </c>
+      <c r="M12">
+        <v>20315</v>
+      </c>
+      <c r="N12">
+        <v>23690</v>
+      </c>
+      <c r="O12">
+        <v>29185</v>
+      </c>
+      <c r="P12">
+        <v>31523</v>
+      </c>
+      <c r="Q12">
+        <v>35125</v>
+      </c>
+      <c r="R12">
+        <v>39547</v>
+      </c>
+      <c r="S12">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <f>AVERAGE(B3:B12)</f>
+        <v>935.4</v>
+      </c>
+      <c r="C13">
+        <f>AVERAGE(C3:C12)</f>
+        <v>1399.4</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:S13" si="0">AVERAGE(D3:D12)</f>
+        <v>2452.4</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>3589.9</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>4911.1000000000004</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>6471</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>8201.9</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>10156.200000000001</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>12303.2</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>14660.8</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>17427.3</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>20446</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>23765.7</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>27623.599999999999</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>31402.5</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>35260.400000000001</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="0"/>
+        <v>39282.9</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="0"/>
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>136</v>
+      </c>
+      <c r="C14">
+        <v>136</v>
+      </c>
+      <c r="D14">
+        <v>136</v>
+      </c>
+      <c r="E14">
+        <v>136</v>
+      </c>
+      <c r="F14">
+        <v>136</v>
+      </c>
+      <c r="G14">
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <v>74</v>
+      </c>
+      <c r="I14">
+        <v>50</v>
+      </c>
+      <c r="J14">
+        <v>47</v>
+      </c>
+      <c r="K14">
+        <v>43</v>
+      </c>
+      <c r="L14">
+        <v>37</v>
+      </c>
+      <c r="M14">
+        <v>30</v>
+      </c>
+      <c r="N14">
+        <v>27</v>
+      </c>
+      <c r="O14">
+        <v>25</v>
+      </c>
+      <c r="P14">
+        <v>24</v>
+      </c>
+      <c r="Q14">
+        <v>17</v>
+      </c>
+      <c r="R14">
+        <v>17</v>
+      </c>
+      <c r="S14">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added in cuda functionality
</commit_message>
<xml_diff>
--- a/coursework 2/code/results.xlsx
+++ b/coursework 2/code/results.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Analysis" sheetId="1" r:id="rId1"/>
     <sheet name="OpenMP" sheetId="2" r:id="rId2"/>
+    <sheet name="CUDA" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="89">
   <si>
     <t>Number of Particles</t>
   </si>
@@ -50,13 +51,264 @@
   <si>
     <t>Framerate</t>
   </si>
+  <si>
+    <t>CUDA</t>
+  </si>
+  <si>
+    <t>Iteration: 1 Time Taken:  18004</t>
+  </si>
+  <si>
+    <t>Iteration: 2 Time Taken:  17973</t>
+  </si>
+  <si>
+    <t>Iteration: 3 Time Taken:  18108</t>
+  </si>
+  <si>
+    <t>Iteration: 4 Time Taken:  17958</t>
+  </si>
+  <si>
+    <t>Iteration: 5 Time Taken:  17912</t>
+  </si>
+  <si>
+    <t>Iteration: 6 Time Taken:  17918</t>
+  </si>
+  <si>
+    <t>Iteration: 7 Time Taken:  17931</t>
+  </si>
+  <si>
+    <t>Iteration: 8 Time Taken:  17924</t>
+  </si>
+  <si>
+    <t>Iteration: 9 Time Taken:  17908</t>
+  </si>
+  <si>
+    <t>Iteration: 1 Time Taken:  16203</t>
+  </si>
+  <si>
+    <t>Iteration: 2 Time Taken:  16234</t>
+  </si>
+  <si>
+    <t>Iteration: 3 Time Taken:  16260</t>
+  </si>
+  <si>
+    <t>Iteration: 4 Time Taken:  16238</t>
+  </si>
+  <si>
+    <t>Iteration: 5 Time Taken:  16240</t>
+  </si>
+  <si>
+    <t>Iteration: 6 Time Taken:  16210</t>
+  </si>
+  <si>
+    <t>Iteration: 7 Time Taken:  16234</t>
+  </si>
+  <si>
+    <t>Iteration: 8 Time Taken:  16220</t>
+  </si>
+  <si>
+    <t>Iteration: 9 Time Taken:  16234</t>
+  </si>
+  <si>
+    <t>Iteration: 1 Time Taken:  14607</t>
+  </si>
+  <si>
+    <t>Iteration: 2 Time Taken:  14626</t>
+  </si>
+  <si>
+    <t>Iteration: 3 Time Taken:  14606</t>
+  </si>
+  <si>
+    <t>Iteration: 4 Time Taken:  14596</t>
+  </si>
+  <si>
+    <t>Iteration: 5 Time Taken:  14610</t>
+  </si>
+  <si>
+    <t>Iteration: 6 Time Taken:  14600</t>
+  </si>
+  <si>
+    <t>Iteration: 7 Time Taken:  14614</t>
+  </si>
+  <si>
+    <t>Iteration: 8 Time Taken:  14616</t>
+  </si>
+  <si>
+    <t>Iteration: 9 Time Taken:  14584</t>
+  </si>
+  <si>
+    <t>Iteration: 1 Time Taken:  13559</t>
+  </si>
+  <si>
+    <t>Iteration: 2 Time Taken:  13562</t>
+  </si>
+  <si>
+    <t>Iteration: 3 Time Taken:  13568</t>
+  </si>
+  <si>
+    <t>Iteration: 4 Time Taken:  13552</t>
+  </si>
+  <si>
+    <t>Iteration: 5 Time Taken:  13585</t>
+  </si>
+  <si>
+    <t>Iteration: 6 Time Taken:  13589</t>
+  </si>
+  <si>
+    <t>Iteration: 7 Time Taken:  13584</t>
+  </si>
+  <si>
+    <t>Iteration: 8 Time Taken:  13571</t>
+  </si>
+  <si>
+    <t>Iteration: 9 Time Taken:  13587</t>
+  </si>
+  <si>
+    <t>Iteration: 2 Time Taken:  12480</t>
+  </si>
+  <si>
+    <t>Iteration: 3 Time Taken:  12473</t>
+  </si>
+  <si>
+    <t>Iteration: 4 Time Taken:  12501</t>
+  </si>
+  <si>
+    <t>Iteration: 5 Time Taken:  12669</t>
+  </si>
+  <si>
+    <t>Iteration: 6 Time Taken:  12567</t>
+  </si>
+  <si>
+    <t>Iteration: 7 Time Taken:  12489</t>
+  </si>
+  <si>
+    <t>Iteration: 8 Time Taken:  12534</t>
+  </si>
+  <si>
+    <t>Iteration: 9 Time Taken:  12485</t>
+  </si>
+  <si>
+    <t>Iteration: 10 Time Taken:  12464</t>
+  </si>
+  <si>
+    <t>Iteration: 1 Time Taken:  10097</t>
+  </si>
+  <si>
+    <t>Iteration: 2 Time Taken:  10068</t>
+  </si>
+  <si>
+    <t>Iteration: 3 Time Taken:  10051</t>
+  </si>
+  <si>
+    <t>Iteration: 4 Time Taken:  10064</t>
+  </si>
+  <si>
+    <t>Iteration: 5 Time Taken:  10094</t>
+  </si>
+  <si>
+    <t>Iteration: 6 Time Taken:  10061</t>
+  </si>
+  <si>
+    <t>Iteration: 7 Time Taken:  10028</t>
+  </si>
+  <si>
+    <t>Iteration: 8 Time Taken:  10033</t>
+  </si>
+  <si>
+    <t>Iteration: 1 Time Taken:  9176</t>
+  </si>
+  <si>
+    <t>Iteration: 2 Time Taken:  9164</t>
+  </si>
+  <si>
+    <t>Iteration: 3 Time Taken:  9190</t>
+  </si>
+  <si>
+    <t>Iteration: 4 Time Taken:  9177</t>
+  </si>
+  <si>
+    <t>Iteration: 5 Time Taken:  9187</t>
+  </si>
+  <si>
+    <t>Iteration: 6 Time Taken:  9179</t>
+  </si>
+  <si>
+    <t>Iteration: 7 Time Taken:  9159</t>
+  </si>
+  <si>
+    <t>Iteration: 8 Time Taken:  9200</t>
+  </si>
+  <si>
+    <t>Iteration: 9 Time Taken:  9200</t>
+  </si>
+  <si>
+    <t>Iteration: 1 Time Taken:  8302</t>
+  </si>
+  <si>
+    <t>Iteration: 2 Time Taken:  8327</t>
+  </si>
+  <si>
+    <t>Iteration: 3 Time Taken:  8312</t>
+  </si>
+  <si>
+    <t>Iteration: 4 Time Taken:  8308</t>
+  </si>
+  <si>
+    <t>Iteration: 5 Time Taken:  8309</t>
+  </si>
+  <si>
+    <t>Iteration: 6 Time Taken:  8263</t>
+  </si>
+  <si>
+    <t>Iteration: 7 Time Taken:  8262</t>
+  </si>
+  <si>
+    <t>Iteration: 8 Time Taken:  8291</t>
+  </si>
+  <si>
+    <t>Iteration: 9 Time Taken:  8272</t>
+  </si>
+  <si>
+    <t>Iteration: 1 Time Taken:  7647</t>
+  </si>
+  <si>
+    <t>Iteration: 2 Time Taken:  7648</t>
+  </si>
+  <si>
+    <t>Iteration: 3 Time Taken:  7653</t>
+  </si>
+  <si>
+    <t>Iteration: 4 Time Taken:  7476</t>
+  </si>
+  <si>
+    <t>Iteration: 5 Time Taken:  7359</t>
+  </si>
+  <si>
+    <t>Iteration: 6 Time Taken:  7402</t>
+  </si>
+  <si>
+    <t>Iteration: 7 Time Taken:  7359</t>
+  </si>
+  <si>
+    <t>Iteration: 8 Time Taken:  7365</t>
+  </si>
+  <si>
+    <t>Iteration: 9 Time Taken:  7337</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -84,8 +336,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -148,7 +401,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -491,7 +743,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1166,7 +1417,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1503,7 +1753,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1846,7 +2095,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8810,8 +9058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T14" sqref="A1:T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9613,4 +9861,779 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>250</v>
+      </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="D2">
+        <v>750</v>
+      </c>
+      <c r="E2">
+        <v>1000</v>
+      </c>
+      <c r="F2">
+        <v>1250</v>
+      </c>
+      <c r="G2">
+        <v>1500</v>
+      </c>
+      <c r="H2">
+        <v>1750</v>
+      </c>
+      <c r="I2">
+        <v>2000</v>
+      </c>
+      <c r="J2">
+        <v>2250</v>
+      </c>
+      <c r="K2">
+        <v>2500</v>
+      </c>
+      <c r="L2">
+        <v>2750</v>
+      </c>
+      <c r="M2">
+        <v>3000</v>
+      </c>
+      <c r="N2">
+        <v>3250</v>
+      </c>
+      <c r="O2">
+        <v>3500</v>
+      </c>
+      <c r="P2">
+        <v>3750</v>
+      </c>
+      <c r="Q2">
+        <v>4000</v>
+      </c>
+      <c r="R2">
+        <v>4250</v>
+      </c>
+      <c r="S2">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>917</v>
+      </c>
+      <c r="C3">
+        <v>1361</v>
+      </c>
+      <c r="D3">
+        <v>2506</v>
+      </c>
+      <c r="E3">
+        <v>3724</v>
+      </c>
+      <c r="F3">
+        <v>4905</v>
+      </c>
+      <c r="G3">
+        <v>6447</v>
+      </c>
+      <c r="H3">
+        <v>8134</v>
+      </c>
+      <c r="I3">
+        <v>10195</v>
+      </c>
+      <c r="J3">
+        <v>7702</v>
+      </c>
+      <c r="K3">
+        <v>8384</v>
+      </c>
+      <c r="L3">
+        <v>9363</v>
+      </c>
+      <c r="M3">
+        <v>10126</v>
+      </c>
+      <c r="O3">
+        <v>12521</v>
+      </c>
+      <c r="P3">
+        <v>13582</v>
+      </c>
+      <c r="Q3">
+        <v>14748</v>
+      </c>
+      <c r="R3">
+        <v>16264</v>
+      </c>
+      <c r="S3" s="1">
+        <v>18043</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>945</v>
+      </c>
+      <c r="C4">
+        <v>1412</v>
+      </c>
+      <c r="D4">
+        <v>2480</v>
+      </c>
+      <c r="E4">
+        <v>3754</v>
+      </c>
+      <c r="F4">
+        <v>4973</v>
+      </c>
+      <c r="G4">
+        <v>6484</v>
+      </c>
+      <c r="H4">
+        <v>8305</v>
+      </c>
+      <c r="I4">
+        <v>10139</v>
+      </c>
+      <c r="J4" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1008</v>
+      </c>
+      <c r="C5">
+        <v>1430</v>
+      </c>
+      <c r="D5">
+        <v>2477</v>
+      </c>
+      <c r="E5">
+        <v>3524</v>
+      </c>
+      <c r="F5">
+        <v>4900</v>
+      </c>
+      <c r="G5">
+        <v>6514</v>
+      </c>
+      <c r="H5">
+        <v>8373</v>
+      </c>
+      <c r="I5">
+        <v>10110</v>
+      </c>
+      <c r="J5" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M5" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>905</v>
+      </c>
+      <c r="C6">
+        <v>1627</v>
+      </c>
+      <c r="D6">
+        <v>2477</v>
+      </c>
+      <c r="E6">
+        <v>3521</v>
+      </c>
+      <c r="F6">
+        <v>4898</v>
+      </c>
+      <c r="G6">
+        <v>6524</v>
+      </c>
+      <c r="H6">
+        <v>8332</v>
+      </c>
+      <c r="I6">
+        <v>10116</v>
+      </c>
+      <c r="J6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L6" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" t="s">
+        <v>20</v>
+      </c>
+      <c r="S6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>929</v>
+      </c>
+      <c r="C7">
+        <v>893</v>
+      </c>
+      <c r="D7">
+        <v>2480</v>
+      </c>
+      <c r="E7">
+        <v>4103</v>
+      </c>
+      <c r="F7">
+        <v>4906</v>
+      </c>
+      <c r="G7">
+        <v>6457</v>
+      </c>
+      <c r="H7">
+        <v>8221</v>
+      </c>
+      <c r="I7">
+        <v>10169</v>
+      </c>
+      <c r="J7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L7" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" t="s">
+        <v>57</v>
+      </c>
+      <c r="O7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R7" t="s">
+        <v>21</v>
+      </c>
+      <c r="S7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>901</v>
+      </c>
+      <c r="C8">
+        <v>733</v>
+      </c>
+      <c r="D8">
+        <v>2397</v>
+      </c>
+      <c r="E8">
+        <v>3472</v>
+      </c>
+      <c r="F8">
+        <v>4911</v>
+      </c>
+      <c r="G8">
+        <v>6424</v>
+      </c>
+      <c r="H8">
+        <v>8133</v>
+      </c>
+      <c r="I8">
+        <v>10075</v>
+      </c>
+      <c r="J8" t="s">
+        <v>84</v>
+      </c>
+      <c r="K8" t="s">
+        <v>75</v>
+      </c>
+      <c r="L8" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>959</v>
+      </c>
+      <c r="C9">
+        <v>1517</v>
+      </c>
+      <c r="D9">
+        <v>2448</v>
+      </c>
+      <c r="E9">
+        <v>3443</v>
+      </c>
+      <c r="F9">
+        <v>4904</v>
+      </c>
+      <c r="G9">
+        <v>6496</v>
+      </c>
+      <c r="H9">
+        <v>8103</v>
+      </c>
+      <c r="I9">
+        <v>10152</v>
+      </c>
+      <c r="J9" t="s">
+        <v>85</v>
+      </c>
+      <c r="K9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L9" t="s">
+        <v>67</v>
+      </c>
+      <c r="M9" t="s">
+        <v>59</v>
+      </c>
+      <c r="O9" t="s">
+        <v>50</v>
+      </c>
+      <c r="P9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>32</v>
+      </c>
+      <c r="R9" t="s">
+        <v>23</v>
+      </c>
+      <c r="S9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>934</v>
+      </c>
+      <c r="C10">
+        <v>1407</v>
+      </c>
+      <c r="D10">
+        <v>2428</v>
+      </c>
+      <c r="E10">
+        <v>3486</v>
+      </c>
+      <c r="F10">
+        <v>4927</v>
+      </c>
+      <c r="G10">
+        <v>6482</v>
+      </c>
+      <c r="H10">
+        <v>8090</v>
+      </c>
+      <c r="I10">
+        <v>10079</v>
+      </c>
+      <c r="J10" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" t="s">
+        <v>77</v>
+      </c>
+      <c r="L10" t="s">
+        <v>68</v>
+      </c>
+      <c r="M10" t="s">
+        <v>60</v>
+      </c>
+      <c r="O10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>33</v>
+      </c>
+      <c r="R10" t="s">
+        <v>24</v>
+      </c>
+      <c r="S10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>948</v>
+      </c>
+      <c r="C11">
+        <v>2129</v>
+      </c>
+      <c r="D11">
+        <v>2462</v>
+      </c>
+      <c r="E11">
+        <v>3423</v>
+      </c>
+      <c r="F11">
+        <v>4886</v>
+      </c>
+      <c r="G11">
+        <v>6428</v>
+      </c>
+      <c r="H11">
+        <v>8173</v>
+      </c>
+      <c r="I11">
+        <v>10091</v>
+      </c>
+      <c r="J11" t="s">
+        <v>87</v>
+      </c>
+      <c r="K11" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" t="s">
+        <v>61</v>
+      </c>
+      <c r="O11" t="s">
+        <v>52</v>
+      </c>
+      <c r="P11" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>34</v>
+      </c>
+      <c r="R11" t="s">
+        <v>25</v>
+      </c>
+      <c r="S11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>908</v>
+      </c>
+      <c r="C12">
+        <v>1485</v>
+      </c>
+      <c r="D12">
+        <v>2369</v>
+      </c>
+      <c r="E12">
+        <v>3449</v>
+      </c>
+      <c r="F12">
+        <v>4901</v>
+      </c>
+      <c r="G12">
+        <v>6454</v>
+      </c>
+      <c r="H12">
+        <v>8155</v>
+      </c>
+      <c r="I12">
+        <v>10436</v>
+      </c>
+      <c r="J12" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" t="s">
+        <v>79</v>
+      </c>
+      <c r="L12" t="s">
+        <v>70</v>
+      </c>
+      <c r="M12">
+        <v>10135</v>
+      </c>
+      <c r="O12" t="s">
+        <v>53</v>
+      </c>
+      <c r="P12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>35</v>
+      </c>
+      <c r="R12" t="s">
+        <v>26</v>
+      </c>
+      <c r="S12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <f>AVERAGE(B3:B12)</f>
+        <v>935.4</v>
+      </c>
+      <c r="C13">
+        <f>AVERAGE(C3:C12)</f>
+        <v>1399.4</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:S13" si="0">AVERAGE(D3:D12)</f>
+        <v>2452.4</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>3589.9</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>4911.1000000000004</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>6471</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>8201.9</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>10156.200000000001</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>7702</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>8384</v>
+      </c>
+      <c r="L13" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N13">
+        <f>AVERAGE(M3:M12)</f>
+        <v>10130.5</v>
+      </c>
+      <c r="O13">
+        <f>AVERAGE(O3:O12)</f>
+        <v>12521</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>13582</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>14748</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="0"/>
+        <v>16264</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="0"/>
+        <v>18043</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>136</v>
+      </c>
+      <c r="C14">
+        <v>136</v>
+      </c>
+      <c r="D14">
+        <v>136</v>
+      </c>
+      <c r="E14">
+        <v>136</v>
+      </c>
+      <c r="F14">
+        <v>136</v>
+      </c>
+      <c r="G14">
+        <v>136</v>
+      </c>
+      <c r="H14">
+        <v>136</v>
+      </c>
+      <c r="I14">
+        <v>136</v>
+      </c>
+      <c r="J14">
+        <v>136</v>
+      </c>
+      <c r="K14">
+        <v>120</v>
+      </c>
+      <c r="L14">
+        <v>107</v>
+      </c>
+      <c r="M14">
+        <v>100</v>
+      </c>
+      <c r="N14">
+        <v>88</v>
+      </c>
+      <c r="O14">
+        <v>80</v>
+      </c>
+      <c r="P14">
+        <v>74</v>
+      </c>
+      <c r="Q14">
+        <v>70</v>
+      </c>
+      <c r="R14">
+        <v>68</v>
+      </c>
+      <c r="S14">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished everything but results
</commit_message>
<xml_diff>
--- a/coursework 2/code/results.xlsx
+++ b/coursework 2/code/results.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40161070\Documents\GitHub\Cps\coursework 2\code\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="OpenMP" sheetId="2" r:id="rId2"/>
     <sheet name="CUDA" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>Number of Particles</t>
   </si>
@@ -55,11 +60,14 @@
   <si>
     <t>Particles</t>
   </si>
+  <si>
+    <t>OpemMP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -118,9 +126,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -171,6 +179,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -180,7 +208,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.10735870516185476"/>
-          <c:y val="0.13930555555555557"/>
+          <c:y val="0.14856481481481484"/>
           <c:w val="0.86486351706036746"/>
           <c:h val="0.72088764946048411"/>
         </c:manualLayout>
@@ -248,7 +276,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>15360.2</c:v>
+                  <c:v>9721.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>15396.2</c:v>
@@ -269,7 +297,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-26DF-4587-A7BE-650327437E0C}"/>
             </c:ext>
@@ -283,7 +311,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="228993280"/>
         <c:axId val="229007360"/>
@@ -440,10 +467,794 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CUDA(</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Speed)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CUDA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>CUDA!$B$2:$S$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3750</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4250</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CUDA!$B$13:$S$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1012.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1780.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2574.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3280.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4044.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4961.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6172.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6890.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7494.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8303</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9199.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10075.700000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10684.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12518.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13573.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14620.7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16233.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17967.900000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-652F-4FFC-B2BC-9710E2C00B52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="379169192"/>
+        <c:axId val="379173784"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="379169192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="379173784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="379173784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="379169192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>CUDA(Frame-Rate)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>CUDA!$B$2:$S$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3750</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4250</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CUDA!$B$14:$S$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CE4C-4A9A-AD32-02455BD3C5FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="379933320"/>
+        <c:axId val="379934632"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="379933320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="379934632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="379934632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="379933320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -495,6 +1306,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -583,7 +1414,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-CC34-47C3-891D-D6CCDF76D0AA}"/>
             </c:ext>
@@ -597,7 +1428,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="229036032"/>
         <c:axId val="229037568"/>
@@ -755,9 +1585,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -817,6 +1647,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -905,7 +1755,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-465C-4113-9571-7EF164F2EDB0}"/>
             </c:ext>
@@ -919,7 +1769,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="229070336"/>
         <c:axId val="229071872"/>
@@ -1078,9 +1927,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1132,6 +1981,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1230,7 +2099,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6749-499A-B5CF-C1D4C25DD136}"/>
             </c:ext>
@@ -1244,7 +2113,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="229104640"/>
         <c:axId val="229106432"/>
@@ -1402,9 +2270,9 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1450,6 +2318,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1548,7 +2436,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B094-4961-A8E4-183432A36009}"/>
             </c:ext>
@@ -1562,7 +2450,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="229135104"/>
         <c:axId val="229136640"/>
@@ -1720,9 +2607,9 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1774,6 +2661,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1869,7 +2776,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4123-4279-AC72-E57980A81030}"/>
             </c:ext>
@@ -1883,7 +2790,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="229157120"/>
         <c:axId val="229179392"/>
@@ -2041,9 +2947,9 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2075,17 +2981,16 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Number of</a:t>
+              <a:t>OpenMP</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Particles (Average Speed)</a:t>
+              <a:t>(Average Speed)</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2253,7 +3158,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7A99-41FF-AC59-8A52A33DA9C5}"/>
             </c:ext>
@@ -2266,9 +3171,24 @@
             <c:strRef>
               <c:f>OpenMP!$B$15:$S$15</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1691.3 5568.2 18290.1 66579.1 154252.3 298452.2</c:v>
+                  <c:v>1691.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5568.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18290.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66579.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>154252.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>298452.2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2349,6 +3269,11 @@
             </c:numLit>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CF95-4CD4-970F-84CAC0C96688}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2358,7 +3283,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="229314944"/>
         <c:axId val="229316480"/>
@@ -2516,9 +3440,9 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2552,7 +3476,7 @@
               <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Number of Particles (Average Frame-rate)</a:t>
+              <a:t>OpenMP(Average Frame-rate)</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB" sz="1400">
               <a:effectLst/>
@@ -2560,7 +3484,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2569,6 +3492,26 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2728,7 +3671,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1A4E-4C9A-AA24-9EC50DF84D85}"/>
             </c:ext>
@@ -2742,7 +3685,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="229328384"/>
         <c:axId val="229329920"/>
@@ -2899,7 +3841,484 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Speed Up</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.40393744531933506"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>OpenMP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>CUDA!$B$19:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CUDA!$B$20:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.6704197530864198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1267969451931714</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5757400237783123</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6624482983818307</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.309338309000861</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.412989802129857</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4707-4FC1-A561-CFFEC6E3F3DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>CUDA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>CUDA!$B$19:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CUDA!$B$21:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.808103485140047</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9789909961412029</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0948772946321617</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5555128886788365</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.5443754279565676</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.464231829474425</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4707-4FC1-A561-CFFEC6E3F3DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="450069728"/>
+        <c:axId val="450064480"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="450069728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="450064480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="450064480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="450069728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3219,6 +4638,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3735,7 +5194,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4251,7 +5710,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4767,7 +6226,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5283,7 +6742,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5799,7 +7258,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6315,7 +7774,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6831,7 +8290,1039 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7536,14 +10027,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>200026</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
@@ -7589,6 +10080,101 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>233362</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>557212</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>252412</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7852,7 +10438,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7862,8 +10448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:G13"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8550,7 +11136,7 @@
         <v>1</v>
       </c>
       <c r="B30">
-        <v>17123</v>
+        <v>9738</v>
       </c>
       <c r="C30">
         <v>15194</v>
@@ -8579,7 +11165,7 @@
         <v>2</v>
       </c>
       <c r="B31">
-        <v>15223</v>
+        <v>9709</v>
       </c>
       <c r="C31">
         <v>15482</v>
@@ -8602,7 +11188,7 @@
         <v>3</v>
       </c>
       <c r="B32">
-        <v>15256</v>
+        <v>9764</v>
       </c>
       <c r="C32">
         <v>16287</v>
@@ -8625,7 +11211,7 @@
         <v>4</v>
       </c>
       <c r="B33">
-        <v>15318</v>
+        <v>9746</v>
       </c>
       <c r="C33">
         <v>16080</v>
@@ -8648,7 +11234,7 @@
         <v>5</v>
       </c>
       <c r="B34">
-        <v>15431</v>
+        <v>9731</v>
       </c>
       <c r="C34">
         <v>15093</v>
@@ -8671,7 +11257,7 @@
         <v>6</v>
       </c>
       <c r="B35">
-        <v>15160</v>
+        <v>9723</v>
       </c>
       <c r="C35">
         <v>15136</v>
@@ -8694,7 +11280,7 @@
         <v>7</v>
       </c>
       <c r="B36">
-        <v>15024</v>
+        <v>9678</v>
       </c>
       <c r="C36">
         <v>15184</v>
@@ -8717,7 +11303,7 @@
         <v>8</v>
       </c>
       <c r="B37">
-        <v>15044</v>
+        <v>9676</v>
       </c>
       <c r="C37">
         <v>15130</v>
@@ -8740,7 +11326,7 @@
         <v>9</v>
       </c>
       <c r="B38">
-        <v>15009</v>
+        <v>9700</v>
       </c>
       <c r="C38">
         <v>15097</v>
@@ -8763,7 +11349,7 @@
         <v>10</v>
       </c>
       <c r="B39">
-        <v>15014</v>
+        <v>9749</v>
       </c>
       <c r="C39">
         <v>15279</v>
@@ -8787,7 +11373,7 @@
       </c>
       <c r="B40">
         <f>AVERAGE(B30:B39)</f>
-        <v>15360.2</v>
+        <v>9721.4</v>
       </c>
       <c r="C40">
         <f t="shared" ref="C40:G40" si="2">AVERAGE(C30:C39)</f>
@@ -8843,8 +11429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:Q16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9714,7 +12300,7 @@
         <v>1.808103485140047</v>
       </c>
       <c r="C37">
-        <f t="shared" ref="C37:G37" si="1">SUM(C15/C13)</f>
+        <f t="shared" ref="C37" si="1">SUM(C15/C13)</f>
         <v>3.9789909961412029</v>
       </c>
       <c r="D37">
@@ -9742,10 +12328,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="A19" sqref="A19:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9821,6 +12407,30 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>1014</v>
+      </c>
+      <c r="C3">
+        <v>1781</v>
+      </c>
+      <c r="D3">
+        <v>2554</v>
+      </c>
+      <c r="E3">
+        <v>3288</v>
+      </c>
+      <c r="F3">
+        <v>4088</v>
+      </c>
+      <c r="G3">
+        <v>4991</v>
+      </c>
+      <c r="H3">
+        <v>6324</v>
+      </c>
+      <c r="I3">
+        <v>6685</v>
+      </c>
       <c r="J3">
         <v>7702</v>
       </c>
@@ -9832,6 +12442,9 @@
       </c>
       <c r="M3">
         <v>10126</v>
+      </c>
+      <c r="N3">
+        <v>10804</v>
       </c>
       <c r="O3">
         <v>12521</v>
@@ -9853,6 +12466,30 @@
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>1015</v>
+      </c>
+      <c r="C4">
+        <v>1806</v>
+      </c>
+      <c r="D4">
+        <v>2542</v>
+      </c>
+      <c r="E4">
+        <v>3283</v>
+      </c>
+      <c r="F4">
+        <v>4034</v>
+      </c>
+      <c r="G4">
+        <v>5016</v>
+      </c>
+      <c r="H4">
+        <v>6655</v>
+      </c>
+      <c r="I4">
+        <v>6726</v>
+      </c>
       <c r="J4">
         <v>7647</v>
       </c>
@@ -9864,6 +12501,9 @@
       </c>
       <c r="M4">
         <v>10097</v>
+      </c>
+      <c r="N4">
+        <v>10729</v>
       </c>
       <c r="O4">
         <v>12480</v>
@@ -9885,6 +12525,30 @@
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>1004</v>
+      </c>
+      <c r="C5">
+        <v>1796</v>
+      </c>
+      <c r="D5">
+        <v>2555</v>
+      </c>
+      <c r="E5">
+        <v>3290</v>
+      </c>
+      <c r="F5">
+        <v>4098</v>
+      </c>
+      <c r="G5">
+        <v>4973</v>
+      </c>
+      <c r="H5">
+        <v>6460</v>
+      </c>
+      <c r="I5">
+        <v>6664</v>
+      </c>
       <c r="J5">
         <v>7648</v>
       </c>
@@ -9896,6 +12560,9 @@
       </c>
       <c r="M5">
         <v>10068</v>
+      </c>
+      <c r="N5">
+        <v>10685</v>
       </c>
       <c r="O5">
         <v>12473</v>
@@ -9917,6 +12584,30 @@
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>1018</v>
+      </c>
+      <c r="C6">
+        <v>1776</v>
+      </c>
+      <c r="D6">
+        <v>2593</v>
+      </c>
+      <c r="E6">
+        <v>3298</v>
+      </c>
+      <c r="F6">
+        <v>4066</v>
+      </c>
+      <c r="G6">
+        <v>4976</v>
+      </c>
+      <c r="H6">
+        <v>6615</v>
+      </c>
+      <c r="I6">
+        <v>6671</v>
+      </c>
       <c r="J6">
         <v>7653</v>
       </c>
@@ -9928,6 +12619,9 @@
       </c>
       <c r="M6">
         <v>10051</v>
+      </c>
+      <c r="N6">
+        <v>10754</v>
       </c>
       <c r="O6">
         <v>12501</v>
@@ -9949,6 +12643,30 @@
       <c r="A7">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>1011</v>
+      </c>
+      <c r="C7">
+        <v>1779</v>
+      </c>
+      <c r="D7">
+        <v>2573</v>
+      </c>
+      <c r="E7">
+        <v>3320</v>
+      </c>
+      <c r="F7">
+        <v>4058</v>
+      </c>
+      <c r="G7">
+        <v>4976</v>
+      </c>
+      <c r="H7">
+        <v>6177</v>
+      </c>
+      <c r="I7">
+        <v>6879</v>
+      </c>
       <c r="J7">
         <v>7476</v>
       </c>
@@ -9960,6 +12678,9 @@
       </c>
       <c r="M7">
         <v>10064</v>
+      </c>
+      <c r="N7">
+        <v>10716</v>
       </c>
       <c r="O7">
         <v>12669</v>
@@ -9981,6 +12702,30 @@
       <c r="A8">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>1017</v>
+      </c>
+      <c r="C8">
+        <v>1777</v>
+      </c>
+      <c r="D8">
+        <v>2553</v>
+      </c>
+      <c r="E8">
+        <v>3288</v>
+      </c>
+      <c r="F8">
+        <v>4019</v>
+      </c>
+      <c r="G8">
+        <v>4942</v>
+      </c>
+      <c r="H8">
+        <v>5966</v>
+      </c>
+      <c r="I8">
+        <v>6819</v>
+      </c>
       <c r="J8">
         <v>7359</v>
       </c>
@@ -9992,6 +12737,9 @@
       </c>
       <c r="M8">
         <v>10094</v>
+      </c>
+      <c r="N8">
+        <v>10714</v>
       </c>
       <c r="O8">
         <v>12567</v>
@@ -10013,6 +12761,30 @@
       <c r="A9">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>1015</v>
+      </c>
+      <c r="C9">
+        <v>1779</v>
+      </c>
+      <c r="D9">
+        <v>2592</v>
+      </c>
+      <c r="E9">
+        <v>3251</v>
+      </c>
+      <c r="F9">
+        <v>3995</v>
+      </c>
+      <c r="G9">
+        <v>4933</v>
+      </c>
+      <c r="H9">
+        <v>6010</v>
+      </c>
+      <c r="I9">
+        <v>6772</v>
+      </c>
       <c r="J9">
         <v>7402</v>
       </c>
@@ -10024,6 +12796,9 @@
       </c>
       <c r="M9">
         <v>10061</v>
+      </c>
+      <c r="N9">
+        <v>10626</v>
       </c>
       <c r="O9">
         <v>12489</v>
@@ -10045,6 +12820,30 @@
       <c r="A10">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>1011</v>
+      </c>
+      <c r="C10">
+        <v>1764</v>
+      </c>
+      <c r="D10">
+        <v>2647</v>
+      </c>
+      <c r="E10">
+        <v>3276</v>
+      </c>
+      <c r="F10">
+        <v>4009</v>
+      </c>
+      <c r="G10">
+        <v>4964</v>
+      </c>
+      <c r="H10">
+        <v>5977</v>
+      </c>
+      <c r="I10">
+        <v>7208</v>
+      </c>
       <c r="J10">
         <v>7359</v>
       </c>
@@ -10056,6 +12855,9 @@
       </c>
       <c r="M10">
         <v>10028</v>
+      </c>
+      <c r="N10">
+        <v>10601</v>
       </c>
       <c r="O10">
         <v>12534</v>
@@ -10077,6 +12879,30 @@
       <c r="A11">
         <v>9</v>
       </c>
+      <c r="B11">
+        <v>1010</v>
+      </c>
+      <c r="C11">
+        <v>1786</v>
+      </c>
+      <c r="D11">
+        <v>2590</v>
+      </c>
+      <c r="E11">
+        <v>3263</v>
+      </c>
+      <c r="F11">
+        <v>4015</v>
+      </c>
+      <c r="G11">
+        <v>4924</v>
+      </c>
+      <c r="H11">
+        <v>5797</v>
+      </c>
+      <c r="I11">
+        <v>7297</v>
+      </c>
       <c r="J11">
         <v>7365</v>
       </c>
@@ -10088,6 +12914,9 @@
       </c>
       <c r="M11">
         <v>10033</v>
+      </c>
+      <c r="N11">
+        <v>10602</v>
       </c>
       <c r="O11">
         <v>12485</v>
@@ -10109,6 +12938,30 @@
       <c r="A12">
         <v>10</v>
       </c>
+      <c r="B12">
+        <v>1010</v>
+      </c>
+      <c r="C12">
+        <v>1764</v>
+      </c>
+      <c r="D12">
+        <v>2545</v>
+      </c>
+      <c r="E12">
+        <v>3246</v>
+      </c>
+      <c r="F12">
+        <v>4067</v>
+      </c>
+      <c r="G12">
+        <v>4923</v>
+      </c>
+      <c r="H12">
+        <v>5745</v>
+      </c>
+      <c r="I12">
+        <v>7184</v>
+      </c>
       <c r="J12">
         <v>7337</v>
       </c>
@@ -10120,6 +12973,9 @@
       </c>
       <c r="M12">
         <v>10135</v>
+      </c>
+      <c r="N12">
+        <v>10610</v>
       </c>
       <c r="O12">
         <v>12464</v>
@@ -10141,37 +12997,37 @@
       <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="B13" t="e">
+      <c r="B13">
         <f>AVERAGE(B3:B12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C13" t="e">
+        <v>1012.5</v>
+      </c>
+      <c r="C13">
         <f>AVERAGE(C3:C12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D13" t="e">
+        <v>1780.8</v>
+      </c>
+      <c r="D13">
         <f t="shared" ref="D13:S13" si="0">AVERAGE(D3:D12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E13" t="e">
+        <v>2574.4</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" t="e">
+        <v>3280.3</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G13" t="e">
+        <v>4044.9</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H13" t="e">
+        <v>4961.8</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I13" t="e">
+        <v>6172.6</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>6890.5</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
@@ -10190,8 +13046,8 @@
         <v>10075.700000000001</v>
       </c>
       <c r="N13">
-        <f>AVERAGE(M3:M12)</f>
-        <v>10075.700000000001</v>
+        <f>AVERAGE(N3:N12)</f>
+        <v>10684.1</v>
       </c>
       <c r="O13">
         <f>AVERAGE(O3:O12)</f>
@@ -10338,23 +13194,23 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="e">
+        <v>8</v>
+      </c>
+      <c r="B20">
         <f>SUM(B15/B13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C20" t="e">
+        <v>1.6704197530864198</v>
+      </c>
+      <c r="C20">
         <f>SUM(C15/C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D20" t="e">
+        <v>3.1267969451931714</v>
+      </c>
+      <c r="D20">
         <f>SUM(E15/E13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E20" t="e">
+        <v>5.5757400237783123</v>
+      </c>
+      <c r="E20">
         <f>SUM(I15/I13)</f>
-        <v>#DIV/0!</v>
+        <v>9.6624482983818307</v>
       </c>
       <c r="F20">
         <f>SUM(M15/M13)</f>
@@ -10363,10 +13219,34 @@
       <c r="G20">
         <f>SUM(Q15/Q13)</f>
         <v>20.412989802129857</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>1.808103485140047</v>
+      </c>
+      <c r="C21">
+        <v>3.9789909961412029</v>
+      </c>
+      <c r="D21">
+        <v>5.0948772946321617</v>
+      </c>
+      <c r="E21">
+        <v>6.5555128886788365</v>
+      </c>
+      <c r="F21">
+        <v>7.5443754279565676</v>
+      </c>
+      <c r="G21">
+        <v>8.464231829474425</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>